<commit_message>
Template da Planilha de Não Conformidades - v1.0
</commit_message>
<xml_diff>
--- a/Documentação/Templates/Template da Planilha de Não Conformidades.xlsx
+++ b/Documentação/Templates/Template da Planilha de Não Conformidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel F\Documents\Faculdade\4º Período\Qualidade de Software\PLANO DE AÇÃO\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meira.gabriel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7026959B-8FBB-46E0-B106-0F3BD12F9603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8433CED-837C-462C-83EA-25817F34D413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C9F11E29-295F-4C42-8910-F24FE80A3C14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9F11E29-295F-4C42-8910-F24FE80A3C14}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -77,13 +77,19 @@
     <t>Avaliador que encontrou a Não Conformidade</t>
   </si>
   <si>
-    <t>Selecionar entre: Baixa-Simples, Baixa-Complexa, Intermediária-Simples, Intermediária-Complexa, Alta-Simples, Alta-Complexa e Muito Complexa.</t>
-  </si>
-  <si>
-    <t>Descrição da Não Conformidade</t>
-  </si>
-  <si>
     <t>COD. NCF</t>
+  </si>
+  <si>
+    <t>MOTIVO</t>
+  </si>
+  <si>
+    <t>Motivo da ocorrência da não conformidade</t>
+  </si>
+  <si>
+    <t>Selecionar entre: Baixa-Simples, Baixa-Complexa, Intermediária-Simples, Intermediária-Complexa, Alta-Simples, Alta-Complexa e Muito Complexa</t>
+  </si>
+  <si>
+    <t>Descrição do requisito que apresenta uma não conformidade</t>
   </si>
 </sst>
 </file>
@@ -119,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -142,11 +148,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -155,10 +181,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,261 +515,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2ECF36F-E193-4851-B203-B728B23C6A6D}">
-  <dimension ref="B2:I21"/>
+  <dimension ref="B2:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B2:J2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>